<commit_message>
Updated input_paramters.xslx and added new test files
New input parameters for more accurate fitting.
</commit_message>
<xml_diff>
--- a/src-experimental/input_parameters.xlsx
+++ b/src-experimental/input_parameters.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25280" yWindow="580" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -532,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -546,19 +546,19 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1100</v>
+        <v>1160</v>
       </c>
       <c r="C3">
-        <v>1250</v>
+        <v>1260</v>
       </c>
       <c r="D3">
         <v>1330</v>
       </c>
       <c r="E3">
-        <v>1420</v>
+        <v>1400</v>
       </c>
       <c r="F3">
-        <v>1500</v>
+        <v>1520</v>
       </c>
       <c r="G3">
         <v>1590</v>
@@ -571,11 +571,23 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
+      <c r="C4">
+        <v>1240</v>
+      </c>
+      <c r="F4">
+        <v>1500</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>17</v>
       </c>
+      <c r="C5">
+        <v>1275</v>
+      </c>
+      <c r="E5">
+        <v>1440</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -633,6 +645,12 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -648,10 +666,10 @@
         <v>5000</v>
       </c>
       <c r="E9">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="F9">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="G9">
         <v>2000</v>

</xml_diff>